<commit_message>
trying to add 45 worker
</commit_message>
<xml_diff>
--- a/BOCW_DETAILS.xlsx
+++ b/BOCW_DETAILS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JAVA\Programm\27-11-2025\src\Dec2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A096A4BE-6683-4654-9059-BC922485615C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E3BE7D-36B0-4D9D-82FC-4A1C66804E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A895EFCD-5E25-4508-B4C3-7FF6155F4E63}"/>
   </bookViews>
@@ -870,11 +870,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED9F30E-840D-4B74-9AEF-B84F532BE371}">
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2754,6 +2754,11 @@
       <c r="N45" s="7"/>
       <c r="O45" s="9" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A46" s="6">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2940,9 +2945,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3090,20 +3098,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCD2CC2D-6F3C-46C6-A6EE-424BCCD4BE8D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C77650B5-CCF3-4EDD-B86A-A6D823D90181}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3128,9 +3131,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C77650B5-CCF3-4EDD-B86A-A6D823D90181}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCD2CC2D-6F3C-46C6-A6EE-424BCCD4BE8D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>